<commit_message>
AShot verified for premier press
</commit_message>
<xml_diff>
--- a/src/test/resources/Documents/24084/Base/JobMaterial.xlsx
+++ b/src/test/resources/Documents/24084/Base/JobMaterial.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="57">
   <si>
     <t>Materialtype</t>
   </si>
@@ -47,42 +47,42 @@
     <t xml:space="preserve">1-Design Jet </t>
   </si>
   <si>
+    <t>Cover Case Bind  4p</t>
+  </si>
+  <si>
+    <t>Print Uncollated F 4x0</t>
+  </si>
+  <si>
+    <t>Design Jet-IS29</t>
+  </si>
+  <si>
+    <t>1.00</t>
+  </si>
+  <si>
+    <t>Ea</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>445 - iQuote - Proofs - Each</t>
+  </si>
+  <si>
+    <t>Text 12p - 1</t>
+  </si>
+  <si>
+    <t>Print Uncollated F/B 4x4</t>
+  </si>
+  <si>
+    <t>Text 12p - 3</t>
+  </si>
+  <si>
     <t>Text  4p</t>
   </si>
   <si>
-    <t>Print Uncollated F/B 4x4</t>
-  </si>
-  <si>
-    <t>Design Jet-IS29</t>
-  </si>
-  <si>
-    <t>1.00</t>
-  </si>
-  <si>
-    <t>Ea</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>445 - iQuote - Proofs - Each</t>
-  </si>
-  <si>
     <t>Text 12p - 2</t>
   </si>
   <si>
-    <t>Cover Case Bind  4p</t>
-  </si>
-  <si>
-    <t>Print Uncollated F 4x0</t>
-  </si>
-  <si>
-    <t>Text 12p - 1</t>
-  </si>
-  <si>
-    <t>Text 12p - 3</t>
-  </si>
-  <si>
     <t>1-Epson Proof</t>
   </si>
   <si>
@@ -113,40 +113,58 @@
     <t>Ink / Varnish</t>
   </si>
   <si>
+    <t xml:space="preserve">Magenta - IS29 Inkjet - </t>
+  </si>
+  <si>
+    <t>0.05</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>449 - iQuote per liter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yellow - IS29 Inkjet - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black - IS29 Inkjet - </t>
+  </si>
+  <si>
     <t xml:space="preserve">Cyan - IS29 Inkjet - </t>
   </si>
   <si>
+    <t>0.21</t>
+  </si>
+  <si>
     <t>0.09</t>
   </si>
   <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>449 - iQuote per liter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magenta - IS29 Inkjet - </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yellow - IS29 Inkjet - </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Black - IS29 Inkjet - </t>
-  </si>
-  <si>
-    <t>0.21</t>
-  </si>
-  <si>
-    <t>0.05</t>
-  </si>
-  <si>
     <t>Sheet</t>
   </si>
   <si>
-    <t>Cougar Opaque Smooth Text White Domtar FSC 100# 19 x 25" 260 ppi</t>
-  </si>
-  <si>
-    <t>372.00</t>
+    <t>End Sheet  4p - 1</t>
+  </si>
+  <si>
+    <t>Cut for Press</t>
+  </si>
+  <si>
+    <t>Special Order Uncoated Cover Non FSC 80# 26 x 40" 210 ppi</t>
+  </si>
+  <si>
+    <t>145.00</t>
+  </si>
+  <si>
+    <t>Sht.</t>
+  </si>
+  <si>
+    <t>429 - Offset Stock cost ea for Jobs Only-Use  for shipping too.</t>
+  </si>
+  <si>
+    <t>Cougar Opaque Smooth Text White Domtar FSC 100# 28 x 40" 260 ppi</t>
+  </si>
+  <si>
+    <t>582.00</t>
   </si>
   <si>
     <t>Sht</t>
@@ -155,37 +173,16 @@
     <t>430 - Offset Stock Per 1000 cost for Jobs Only</t>
   </si>
   <si>
-    <t>Cut for Press</t>
+    <t>189.00</t>
+  </si>
+  <si>
+    <t>End Sheet  4p - 2</t>
   </si>
   <si>
     <t>Sterling Ultra C1S Gloss Verso Non FSC 100# 28 x 40" 400 ppi</t>
   </si>
   <si>
     <t>383.00</t>
-  </si>
-  <si>
-    <t>Cougar Opaque Smooth Text White Domtar FSC 100# 23 x 35" 260 ppi</t>
-  </si>
-  <si>
-    <t>582.00</t>
-  </si>
-  <si>
-    <t>End Sheet  4p - 2</t>
-  </si>
-  <si>
-    <t>Special Order Uncoated Cover Non FSC 80# 26 x 40" 210 ppi</t>
-  </si>
-  <si>
-    <t>145.00</t>
-  </si>
-  <si>
-    <t>Sht.</t>
-  </si>
-  <si>
-    <t>429 - Offset Stock cost ea for Jobs Only-Use  for shipping too.</t>
-  </si>
-  <si>
-    <t>End Sheet  4p - 1</t>
   </si>
 </sst>
 </file>
@@ -2132,7 +2129,7 @@
         <v>18</v>
       </c>
       <c r="C3" t="s" s="12">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s" s="13">
         <v>13</v>
@@ -2155,10 +2152,10 @@
         <v>10</v>
       </c>
       <c r="B4" t="s" s="19">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s" s="20">
         <v>19</v>
-      </c>
-      <c r="C4" t="s" s="20">
-        <v>20</v>
       </c>
       <c r="D4" t="s" s="21">
         <v>13</v>
@@ -2184,7 +2181,7 @@
         <v>21</v>
       </c>
       <c r="C5" t="s" s="28">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s" s="29">
         <v>13</v>
@@ -2210,7 +2207,7 @@
         <v>22</v>
       </c>
       <c r="C6" t="s" s="36">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s" s="37">
         <v>13</v>
@@ -2242,7 +2239,7 @@
         <v>24</v>
       </c>
       <c r="E7" t="s" s="46">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s" s="47">
         <v>15</v>
@@ -2262,7 +2259,7 @@
         <v>18</v>
       </c>
       <c r="C8" t="s" s="52">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s" s="53">
         <v>24</v>
@@ -2285,16 +2282,16 @@
         <v>23</v>
       </c>
       <c r="B9" t="s" s="59">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s" s="60">
         <v>19</v>
-      </c>
-      <c r="C9" t="s" s="60">
-        <v>20</v>
       </c>
       <c r="D9" t="s" s="61">
         <v>24</v>
       </c>
       <c r="E9" t="s" s="62">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s" s="63">
         <v>15</v>
@@ -2314,7 +2311,7 @@
         <v>21</v>
       </c>
       <c r="C10" t="s" s="68">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s" s="69">
         <v>24</v>
@@ -2340,7 +2337,7 @@
         <v>22</v>
       </c>
       <c r="C11" t="s" s="76">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s" s="77">
         <v>24</v>
@@ -2496,10 +2493,10 @@
         <v>18</v>
       </c>
       <c r="C17" t="s" s="124">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D17" t="s" s="125">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E17" t="s" s="126">
         <v>40</v>
@@ -2522,10 +2519,10 @@
         <v>18</v>
       </c>
       <c r="C18" t="s" s="132">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D18" t="s" s="133">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s" s="134">
         <v>40</v>
@@ -2548,10 +2545,10 @@
         <v>18</v>
       </c>
       <c r="C19" t="s" s="140">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D19" t="s" s="141">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E19" t="s" s="142">
         <v>40</v>
@@ -2574,10 +2571,10 @@
         <v>18</v>
       </c>
       <c r="C20" t="s" s="148">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D20" t="s" s="149">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E20" t="s" s="150">
         <v>40</v>
@@ -2597,16 +2594,16 @@
         <v>32</v>
       </c>
       <c r="B21" t="s" s="155">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s" s="156">
         <v>19</v>
       </c>
-      <c r="C21" t="s" s="156">
-        <v>20</v>
-      </c>
       <c r="D21" t="s" s="157">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E21" t="s" s="158">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F21" t="s" s="159">
         <v>35</v>
@@ -2623,16 +2620,16 @@
         <v>32</v>
       </c>
       <c r="B22" t="s" s="163">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s" s="164">
         <v>19</v>
       </c>
-      <c r="C22" t="s" s="164">
-        <v>20</v>
-      </c>
       <c r="D22" t="s" s="165">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E22" t="s" s="166">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F22" t="s" s="167">
         <v>35</v>
@@ -2649,16 +2646,16 @@
         <v>32</v>
       </c>
       <c r="B23" t="s" s="171">
+        <v>20</v>
+      </c>
+      <c r="C23" t="s" s="172">
         <v>19</v>
       </c>
-      <c r="C23" t="s" s="172">
-        <v>20</v>
-      </c>
       <c r="D23" t="s" s="173">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E23" t="s" s="174">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F23" t="s" s="175">
         <v>35</v>
@@ -2675,16 +2672,16 @@
         <v>32</v>
       </c>
       <c r="B24" t="s" s="179">
+        <v>20</v>
+      </c>
+      <c r="C24" t="s" s="180">
         <v>19</v>
       </c>
-      <c r="C24" t="s" s="180">
-        <v>20</v>
-      </c>
       <c r="D24" t="s" s="181">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E24" t="s" s="182">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F24" t="s" s="183">
         <v>35</v>
@@ -2704,13 +2701,13 @@
         <v>21</v>
       </c>
       <c r="C25" t="s" s="188">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D25" t="s" s="189">
         <v>39</v>
       </c>
       <c r="E25" t="s" s="190">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F25" t="s" s="191">
         <v>35</v>
@@ -2730,13 +2727,13 @@
         <v>21</v>
       </c>
       <c r="C26" t="s" s="196">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D26" t="s" s="197">
         <v>37</v>
       </c>
       <c r="E26" t="s" s="198">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F26" t="s" s="199">
         <v>35</v>
@@ -2756,13 +2753,13 @@
         <v>21</v>
       </c>
       <c r="C27" t="s" s="204">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D27" t="s" s="205">
         <v>38</v>
       </c>
       <c r="E27" t="s" s="206">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F27" t="s" s="207">
         <v>35</v>
@@ -2782,13 +2779,13 @@
         <v>21</v>
       </c>
       <c r="C28" t="s" s="212">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D28" t="s" s="213">
         <v>33</v>
       </c>
       <c r="E28" t="s" s="214">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F28" t="s" s="215">
         <v>35</v>
@@ -2808,10 +2805,10 @@
         <v>22</v>
       </c>
       <c r="C29" t="s" s="220">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D29" t="s" s="221">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E29" t="s" s="222">
         <v>40</v>
@@ -2834,10 +2831,10 @@
         <v>22</v>
       </c>
       <c r="C30" t="s" s="228">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D30" t="s" s="229">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E30" t="s" s="230">
         <v>40</v>
@@ -2860,10 +2857,10 @@
         <v>22</v>
       </c>
       <c r="C31" t="s" s="236">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D31" t="s" s="237">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E31" t="s" s="238">
         <v>40</v>
@@ -2886,10 +2883,10 @@
         <v>22</v>
       </c>
       <c r="C32" t="s" s="244">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D32" t="s" s="245">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E32" t="s" s="246">
         <v>40</v>
@@ -2909,25 +2906,25 @@
         <v>42</v>
       </c>
       <c r="B33" t="s" s="251">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="C33" t="s" s="252">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="D33" t="s" s="253">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E33" t="s" s="254">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F33" t="s" s="255">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G33" t="s" s="256">
         <v>16</v>
       </c>
       <c r="H33" t="s" s="257">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34">
@@ -2935,25 +2932,25 @@
         <v>42</v>
       </c>
       <c r="B34" t="s" s="259">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C34" t="s" s="260">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D34" t="s" s="261">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E34" t="s" s="262">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F34" t="s" s="263">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G34" t="s" s="264">
         <v>16</v>
       </c>
       <c r="H34" t="s" s="265">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35">
@@ -2961,25 +2958,25 @@
         <v>42</v>
       </c>
       <c r="B35" t="s" s="267">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C35" t="s" s="268">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D35" t="s" s="269">
+        <v>49</v>
+      </c>
+      <c r="E35" t="s" s="270">
         <v>50</v>
       </c>
-      <c r="E35" t="s" s="270">
+      <c r="F35" t="s" s="271">
         <v>51</v>
       </c>
-      <c r="F35" t="s" s="271">
-        <v>45</v>
-      </c>
       <c r="G35" t="s" s="272">
         <v>16</v>
       </c>
       <c r="H35" t="s" s="273">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36">
@@ -2987,25 +2984,25 @@
         <v>42</v>
       </c>
       <c r="B36" t="s" s="275">
+        <v>21</v>
+      </c>
+      <c r="C36" t="s" s="276">
+        <v>44</v>
+      </c>
+      <c r="D36" t="s" s="277">
+        <v>49</v>
+      </c>
+      <c r="E36" t="s" s="278">
+        <v>53</v>
+      </c>
+      <c r="F36" t="s" s="279">
+        <v>51</v>
+      </c>
+      <c r="G36" t="s" s="280">
+        <v>16</v>
+      </c>
+      <c r="H36" t="s" s="281">
         <v>52</v>
-      </c>
-      <c r="C36" t="s" s="276">
-        <v>47</v>
-      </c>
-      <c r="D36" t="s" s="277">
-        <v>53</v>
-      </c>
-      <c r="E36" t="s" s="278">
-        <v>54</v>
-      </c>
-      <c r="F36" t="s" s="279">
-        <v>55</v>
-      </c>
-      <c r="G36" t="s" s="280">
-        <v>16</v>
-      </c>
-      <c r="H36" t="s" s="281">
-        <v>56</v>
       </c>
     </row>
     <row r="37">
@@ -3016,22 +3013,22 @@
         <v>22</v>
       </c>
       <c r="C37" t="s" s="284">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D37" t="s" s="285">
+        <v>49</v>
+      </c>
+      <c r="E37" t="s" s="286">
         <v>50</v>
       </c>
-      <c r="E37" t="s" s="286">
+      <c r="F37" t="s" s="287">
         <v>51</v>
       </c>
-      <c r="F37" t="s" s="287">
-        <v>45</v>
-      </c>
       <c r="G37" t="s" s="288">
         <v>16</v>
       </c>
       <c r="H37" t="s" s="289">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38">
@@ -3039,25 +3036,25 @@
         <v>42</v>
       </c>
       <c r="B38" t="s" s="291">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C38" t="s" s="292">
+        <v>44</v>
+      </c>
+      <c r="D38" t="s" s="293">
+        <v>45</v>
+      </c>
+      <c r="E38" t="s" s="294">
+        <v>46</v>
+      </c>
+      <c r="F38" t="s" s="295">
         <v>47</v>
       </c>
-      <c r="D38" t="s" s="293">
-        <v>53</v>
-      </c>
-      <c r="E38" t="s" s="294">
-        <v>54</v>
-      </c>
-      <c r="F38" t="s" s="295">
-        <v>55</v>
-      </c>
       <c r="G38" t="s" s="296">
         <v>16</v>
       </c>
       <c r="H38" t="s" s="297">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39">
@@ -3065,25 +3062,25 @@
         <v>42</v>
       </c>
       <c r="B39" t="s" s="299">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C39" t="s" s="300">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D39" t="s" s="301">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E39" t="s" s="302">
+        <v>56</v>
+      </c>
+      <c r="F39" t="s" s="303">
         <v>51</v>
       </c>
-      <c r="F39" t="s" s="303">
-        <v>45</v>
-      </c>
       <c r="G39" t="s" s="304">
         <v>16</v>
       </c>
       <c r="H39" t="s" s="305">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>